<commit_message>
Update Aplikasi tgl 31-10-19
</commit_message>
<xml_diff>
--- a/assets/file_format/import_employee.xlsx
+++ b/assets/file_format/import_employee.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="8940"/>
+    <workbookView windowWidth="21863" windowHeight="9804"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>NIP</t>
   </si>
@@ -152,76 +152,43 @@
     <t>hris</t>
   </si>
   <si>
-    <t>ISMAIL</t>
-  </si>
-  <si>
-    <t>MAIL</t>
-  </si>
-  <si>
-    <t>Laki-Laki</t>
+    <t>SUGENG SUKANTO</t>
+  </si>
+  <si>
+    <t>SUGENG</t>
   </si>
   <si>
     <t>AB</t>
   </si>
   <si>
-    <t>SMP PUTRA</t>
-  </si>
-  <si>
-    <t>JL KEMENANGAN V</t>
-  </si>
-  <si>
-    <t>jakarta barat</t>
-  </si>
-  <si>
-    <t>tamansari</t>
-  </si>
-  <si>
-    <t>ndrianggar@gmail.com</t>
-  </si>
-  <si>
-    <t>kuningan</t>
-  </si>
-  <si>
-    <t>32112332323232</t>
-  </si>
-  <si>
-    <t>231321323232321</t>
+    <t>sfmsadfas</t>
+  </si>
+  <si>
+    <t>Cijantung</t>
+  </si>
+  <si>
+    <t>Pasar Rebo</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>ANISARAH, S.Pd</t>
+  </si>
+  <si>
+    <t>ANI</t>
+  </si>
+  <si>
+    <t>SATWIKA PARAMA NANDINI</t>
+  </si>
+  <si>
+    <t>WIKA</t>
+  </si>
+  <si>
+    <t>akademik</t>
   </si>
   <si>
     <t>Nikah</t>
-  </si>
-  <si>
-    <t>Ruki</t>
-  </si>
-  <si>
-    <t>30,20</t>
-  </si>
-  <si>
-    <t>02197600722</t>
-  </si>
-  <si>
-    <t>Rusmani</t>
-  </si>
-  <si>
-    <t>Rusman</t>
-  </si>
-  <si>
-    <t>321345465233212</t>
-  </si>
-  <si>
-    <t>DIV0001</t>
-  </si>
-  <si>
-    <t>CBG00001</t>
-  </si>
-  <si>
-    <t>akademik</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
   </si>
   <si>
     <t>Duda/Janda</t>
@@ -233,9 +200,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -272,6 +239,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -279,15 +253,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,7 +283,54 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,77 +344,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,19 +389,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +509,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,139 +551,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,21 +588,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,17 +616,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,8 +628,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,170 +660,180 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -880,7 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,13 +1166,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AN13" sqref="AN13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="11.6666666666667" customWidth="1"/>
@@ -1385,10 +1351,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
-      <c r="A2">
-        <v>203333333</v>
-      </c>
+    <row r="2" spans="2:34">
       <c r="B2">
         <v>12345</v>
       </c>
@@ -1396,10 +1359,10 @@
         <v>44</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -1410,119 +1373,38 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
       </c>
       <c r="M2">
         <v>3</v>
       </c>
       <c r="N2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="3"/>
+      <c r="U2" s="4">
+        <v>40341</v>
+      </c>
+      <c r="Y2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q2">
-        <v>11120</v>
-      </c>
-      <c r="R2">
-        <v>323232321</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" s="4">
-        <v>33201</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2">
-        <v>2</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>3</v>
-      </c>
-      <c r="AE2">
-        <v>2019</v>
-      </c>
-      <c r="AF2">
-        <v>30</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AI2">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP2">
-        <v>46546565564</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR2">
-        <v>12</v>
-      </c>
+      <c r="AB2" s="4"/>
+      <c r="AH2" s="4"/>
     </row>
-    <row r="3" spans="1:44">
-      <c r="A3">
-        <v>12365489</v>
-      </c>
+    <row r="3" spans="2:25">
       <c r="B3">
         <v>12345</v>
       </c>
@@ -1530,145 +1412,110 @@
         <v>44</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>48</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
         <v>49</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>50</v>
       </c>
-      <c r="M3">
+      <c r="U3" s="4">
+        <v>40342</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25">
+      <c r="B4">
+        <v>12345</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="N3">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>6</v>
+      </c>
+      <c r="O4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="4">
+        <v>40343</v>
+      </c>
+      <c r="Y4" t="s">
         <v>51</v>
-      </c>
-      <c r="P3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3">
-        <v>11120</v>
-      </c>
-      <c r="R3">
-        <v>323232321</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="4">
-        <v>33201</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z3">
-        <v>2</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AC3">
-        <v>1</v>
-      </c>
-      <c r="AD3">
-        <v>3</v>
-      </c>
-      <c r="AE3">
-        <v>2019</v>
-      </c>
-      <c r="AF3">
-        <v>30</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>43793</v>
-      </c>
-      <c r="AI3">
-        <v>3</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP3">
-        <v>46546565564</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR3">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2 C3 C4">
       <formula1>SOURCE!$E$4:$E$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2 I3 I4">
       <formula1>SOURCE!$D$4:$D$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2 Y3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y4">
       <formula1>SOURCE!$F$4:$F$6</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="S2" r:id="rId1" display="ndrianggar@gmail.com"/>
-    <hyperlink ref="S3" r:id="rId1" display="ndrianggar@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1680,7 +1527,7 @@
   <dimension ref="D4:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1689,19 +1536,19 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:6">
-      <c r="D4" t="s">
-        <v>47</v>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="4:6">
-      <c r="D5" t="s">
-        <v>68</v>
+      <c r="D5">
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
@@ -1712,7 +1559,7 @@
     </row>
     <row r="6" spans="6:6">
       <c r="F6" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>